<commit_message>
Adding plots and removing a study from animal behaviour, not really a psychology journal (no large changes in results), and adding to the write up/
</commit_message>
<xml_diff>
--- a/PowerEstimationReviewDataCollection2018.03.05.xlsx
+++ b/PowerEstimationReviewDataCollection2018.03.05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Systematic Reviews\History of Power Estimation Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCF85C7-7F6C-49D7-9EE5-948D28F9AE50}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C927C-96C6-43A4-B15D-B50235816C4A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="10640" windowHeight="5720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="465" windowWidth="10635" windowHeight="5715" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_power_estimates" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,15 @@
     <definedName name="_Hlk504467761" localSheetId="7">'Search terms'!$A$1</definedName>
     <definedName name="PowerEstimationStudiesLib_for_export" localSheetId="4">Randomisation_original_sample!$A$2:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="1208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="1208">
   <si>
     <t>Author</t>
   </si>
@@ -3738,7 +3743,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4200,48 +4205,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="54" zoomScaleNormal="47" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="47" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="47.7890625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="3" max="3" width="47.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.2890625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.9140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.9140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="23.875" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="22.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="32.20703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.20703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.70703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7890625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7890625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.95703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="32.25" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5.625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.25" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.75" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.75" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.75" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.9140625" style="9" customWidth="1"/>
-    <col min="22" max="23" width="10.83203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="9" customWidth="1"/>
-    <col min="25" max="26" width="10.83203125" style="7" customWidth="1"/>
-    <col min="27" max="27" width="10.83203125" style="9" customWidth="1"/>
-    <col min="28" max="32" width="10.83203125" style="7" customWidth="1"/>
-    <col min="33" max="35" width="10.83203125" style="1" customWidth="1"/>
-    <col min="36" max="36" width="10.83203125" style="9" customWidth="1"/>
-    <col min="37" max="40" width="10.83203125" style="1" customWidth="1"/>
-    <col min="41" max="41" width="10.83203125" style="1"/>
-    <col min="42" max="50" width="10.83203125" style="1" customWidth="1"/>
-    <col min="51" max="56" width="10.83203125" style="1"/>
-    <col min="57" max="57" width="41.9140625" style="1" customWidth="1"/>
-    <col min="58" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="14.875" style="9" customWidth="1"/>
+    <col min="22" max="23" width="10.875" style="7" customWidth="1"/>
+    <col min="24" max="24" width="10.875" style="9" customWidth="1"/>
+    <col min="25" max="26" width="10.875" style="7" customWidth="1"/>
+    <col min="27" max="27" width="10.875" style="9" customWidth="1"/>
+    <col min="28" max="32" width="10.875" style="7" customWidth="1"/>
+    <col min="33" max="35" width="10.875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="10.875" style="9" customWidth="1"/>
+    <col min="37" max="40" width="10.875" style="1" customWidth="1"/>
+    <col min="41" max="41" width="10.875" style="1"/>
+    <col min="42" max="50" width="10.875" style="1" customWidth="1"/>
+    <col min="51" max="56" width="10.875" style="1"/>
+    <col min="57" max="57" width="41.875" style="1" customWidth="1"/>
+    <col min="58" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>414</v>
       </c>
@@ -4411,7 +4416,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -4438,7 +4443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -4528,7 +4533,7 @@
       </c>
       <c r="AS3" s="4"/>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>49</v>
       </c>
@@ -4591,7 +4596,7 @@
       </c>
       <c r="AS4" s="4"/>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>60</v>
       </c>
@@ -4700,7 +4705,7 @@
       <c r="AS5" s="4"/>
       <c r="BF5" s="7"/>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>77</v>
       </c>
@@ -4799,7 +4804,7 @@
       </c>
       <c r="AS6" s="4"/>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>77</v>
       </c>
@@ -4884,7 +4889,7 @@
       <c r="AO7" s="4"/>
       <c r="AS7" s="4"/>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -4969,7 +4974,7 @@
       <c r="AO8" s="4"/>
       <c r="AS8" s="4"/>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>77</v>
       </c>
@@ -5054,7 +5059,7 @@
       <c r="AO9" s="4"/>
       <c r="AS9" s="4"/>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>77</v>
       </c>
@@ -5139,7 +5144,7 @@
       <c r="AO10" s="4"/>
       <c r="AS10" s="4"/>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>69</v>
       </c>
@@ -5155,6 +5160,9 @@
       <c r="E11" s="1">
         <v>2011</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>415</v>
       </c>
@@ -5208,7 +5216,7 @@
       </c>
       <c r="AS11" s="4"/>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>69</v>
       </c>
@@ -5218,6 +5226,9 @@
       <c r="E12" s="1">
         <v>2011</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>415</v>
       </c>
@@ -5270,7 +5281,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>69</v>
       </c>
@@ -5280,6 +5291,9 @@
       <c r="E13" s="1">
         <v>2011</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>415</v>
       </c>
@@ -5332,7 +5346,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>109</v>
       </c>
@@ -5403,7 +5417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>46</v>
       </c>
@@ -5429,7 +5443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>84</v>
       </c>
@@ -5455,7 +5469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:58">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>63</v>
       </c>
@@ -5517,7 +5531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:58">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>74</v>
       </c>
@@ -5603,7 +5617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:58">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>107</v>
       </c>
@@ -5716,7 +5730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:58">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>71</v>
       </c>
@@ -5838,7 +5852,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="21" spans="1:58">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>113</v>
       </c>
@@ -5906,7 +5920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:58">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>66</v>
       </c>
@@ -5983,7 +5997,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="23" spans="1:58">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>53</v>
       </c>
@@ -6009,7 +6023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:58">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -6098,7 +6112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="1:58">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>54</v>
       </c>
@@ -6145,7 +6159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:58">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>102</v>
       </c>
@@ -6250,7 +6264,7 @@
       </c>
       <c r="BF26" s="11"/>
     </row>
-    <row r="27" spans="1:58">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>90</v>
       </c>
@@ -6290,7 +6304,7 @@
       <c r="BE27" s="7"/>
       <c r="BF27" s="11"/>
     </row>
-    <row r="28" spans="1:58">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>61</v>
       </c>
@@ -6333,7 +6347,7 @@
       <c r="BE28" s="7"/>
       <c r="BF28" s="11"/>
     </row>
-    <row r="29" spans="1:58">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>86</v>
       </c>
@@ -6420,7 +6434,7 @@
       </c>
       <c r="BF29" s="11"/>
     </row>
-    <row r="30" spans="1:58">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>57</v>
       </c>
@@ -6496,7 +6510,7 @@
       <c r="BE30" s="7"/>
       <c r="BF30" s="11"/>
     </row>
-    <row r="31" spans="1:58">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>57</v>
       </c>
@@ -6563,7 +6577,7 @@
       <c r="BE31" s="7"/>
       <c r="BF31" s="11"/>
     </row>
-    <row r="32" spans="1:58">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -6631,7 +6645,7 @@
       <c r="BE32" s="7"/>
       <c r="BF32" s="11"/>
     </row>
-    <row r="33" spans="1:58">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>57</v>
       </c>
@@ -6699,7 +6713,7 @@
       <c r="BE33" s="7"/>
       <c r="BF33" s="11"/>
     </row>
-    <row r="34" spans="1:58">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>57</v>
       </c>
@@ -6767,7 +6781,7 @@
       <c r="BE34" s="7"/>
       <c r="BF34" s="11"/>
     </row>
-    <row r="35" spans="1:58">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>57</v>
       </c>
@@ -6835,7 +6849,7 @@
       <c r="BE35" s="7"/>
       <c r="BF35" s="11"/>
     </row>
-    <row r="36" spans="1:58">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>78</v>
       </c>
@@ -6915,7 +6929,7 @@
       <c r="BE36" s="7"/>
       <c r="BF36" s="11"/>
     </row>
-    <row r="37" spans="1:58">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>64</v>
       </c>
@@ -6982,7 +6996,7 @@
       <c r="BE37" s="7"/>
       <c r="BF37" s="11"/>
     </row>
-    <row r="38" spans="1:58">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>68</v>
       </c>
@@ -7102,7 +7116,7 @@
       </c>
       <c r="BF38" s="11"/>
     </row>
-    <row r="39" spans="1:58">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>93</v>
       </c>
@@ -7172,7 +7186,7 @@
       <c r="BE39" s="7"/>
       <c r="BF39" s="11"/>
     </row>
-    <row r="40" spans="1:58">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>48</v>
       </c>
@@ -7239,7 +7253,7 @@
       <c r="BE40" s="7"/>
       <c r="BF40" s="11"/>
     </row>
-    <row r="41" spans="1:58">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>48</v>
       </c>
@@ -7285,7 +7299,7 @@
       <c r="BE41" s="7"/>
       <c r="BF41" s="11"/>
     </row>
-    <row r="42" spans="1:58" s="11" customFormat="1">
+    <row r="42" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>88</v>
       </c>
@@ -7387,7 +7401,7 @@
       </c>
       <c r="AJ42" s="14"/>
     </row>
-    <row r="43" spans="1:58" s="11" customFormat="1">
+    <row r="43" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>111</v>
       </c>
@@ -7449,7 +7463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:58" s="11" customFormat="1">
+    <row r="44" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>111</v>
       </c>
@@ -7499,7 +7513,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="45" spans="1:58" s="11" customFormat="1">
+    <row r="45" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>111</v>
       </c>
@@ -7549,7 +7563,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="46" spans="1:58" s="11" customFormat="1">
+    <row r="46" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>111</v>
       </c>
@@ -7599,7 +7613,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="47" spans="1:58" s="11" customFormat="1">
+    <row r="47" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>111</v>
       </c>
@@ -7649,7 +7663,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="48" spans="1:58" s="11" customFormat="1">
+    <row r="48" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>56</v>
       </c>
@@ -7679,7 +7693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:58" s="11" customFormat="1">
+    <row r="49" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>82</v>
       </c>
@@ -7709,7 +7723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:58" s="11" customFormat="1">
+    <row r="50" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>104</v>
       </c>
@@ -7796,7 +7810,7 @@
       </c>
       <c r="AJ50" s="14"/>
     </row>
-    <row r="51" spans="1:58" s="11" customFormat="1">
+    <row r="51" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>87</v>
       </c>
@@ -7826,7 +7840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:58" s="11" customFormat="1">
+    <row r="52" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -7918,7 +7932,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="53" spans="1:58" s="11" customFormat="1">
+    <row r="53" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>67</v>
       </c>
@@ -8030,7 +8044,7 @@
       <c r="AP53" s="1"/>
       <c r="AQ53" s="1"/>
     </row>
-    <row r="54" spans="1:58">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>96</v>
       </c>
@@ -8099,7 +8113,7 @@
       </c>
       <c r="BF54" s="11"/>
     </row>
-    <row r="55" spans="1:58">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>98</v>
       </c>
@@ -8177,7 +8191,7 @@
       </c>
       <c r="BF55" s="11"/>
     </row>
-    <row r="56" spans="1:58">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>79</v>
       </c>
@@ -8244,7 +8258,7 @@
       <c r="BE56" s="7"/>
       <c r="BF56" s="11"/>
     </row>
-    <row r="57" spans="1:58">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>79</v>
       </c>
@@ -8302,7 +8316,7 @@
       <c r="BE57" s="7"/>
       <c r="BF57" s="11"/>
     </row>
-    <row r="58" spans="1:58">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>79</v>
       </c>
@@ -8360,7 +8374,7 @@
       <c r="BE58" s="7"/>
       <c r="BF58" s="11"/>
     </row>
-    <row r="59" spans="1:58">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>79</v>
       </c>
@@ -8418,7 +8432,7 @@
       <c r="BE59" s="7"/>
       <c r="BF59" s="11"/>
     </row>
-    <row r="60" spans="1:58">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>41</v>
       </c>
@@ -8476,7 +8490,7 @@
       <c r="BE60" s="7"/>
       <c r="BF60" s="11"/>
     </row>
-    <row r="61" spans="1:58">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>41</v>
       </c>
@@ -8525,7 +8539,7 @@
       <c r="BE61" s="7"/>
       <c r="BF61" s="7"/>
     </row>
-    <row r="62" spans="1:58">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>106</v>
       </c>
@@ -8630,7 +8644,7 @@
       </c>
       <c r="BF62" s="11"/>
     </row>
-    <row r="63" spans="1:58">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>99</v>
       </c>
@@ -8710,7 +8724,7 @@
       </c>
       <c r="BF63" s="11"/>
     </row>
-    <row r="64" spans="1:58">
+    <row r="64" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>94</v>
       </c>
@@ -8780,7 +8794,7 @@
       <c r="BE64" s="7"/>
       <c r="BF64" s="11"/>
     </row>
-    <row r="65" spans="1:58">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>51</v>
       </c>
@@ -8802,7 +8816,7 @@
       <c r="X65" s="14"/>
       <c r="BF65" s="11"/>
     </row>
-    <row r="66" spans="1:58">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>95</v>
       </c>
@@ -8834,7 +8848,7 @@
       <c r="BE66" s="7"/>
       <c r="BF66" s="11"/>
     </row>
-    <row r="67" spans="1:58">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>85</v>
       </c>
@@ -8875,7 +8889,7 @@
       <c r="BE67" s="7"/>
       <c r="BF67" s="11"/>
     </row>
-    <row r="68" spans="1:58">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>110</v>
       </c>
@@ -8903,7 +8917,7 @@
       <c r="BE68" s="7"/>
       <c r="BF68" s="11"/>
     </row>
-    <row r="69" spans="1:58">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>73</v>
       </c>
@@ -8969,7 +8983,7 @@
       </c>
       <c r="BF69" s="11"/>
     </row>
-    <row r="70" spans="1:58">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>73</v>
       </c>
@@ -9029,7 +9043,7 @@
       </c>
       <c r="BF70" s="7"/>
     </row>
-    <row r="71" spans="1:58">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>80</v>
       </c>
@@ -9057,7 +9071,7 @@
       <c r="BE71" s="7"/>
       <c r="BF71" s="11"/>
     </row>
-    <row r="72" spans="1:58">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>52</v>
       </c>
@@ -9085,7 +9099,7 @@
       <c r="BE72" s="7"/>
       <c r="BF72" s="11"/>
     </row>
-    <row r="73" spans="1:58">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>83</v>
       </c>
@@ -9155,7 +9169,7 @@
       <c r="BE73" s="7"/>
       <c r="BF73" s="11"/>
     </row>
-    <row r="74" spans="1:58">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>91</v>
       </c>
@@ -9230,7 +9244,7 @@
       </c>
       <c r="BF74" s="11"/>
     </row>
-    <row r="75" spans="1:58">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>72</v>
       </c>
@@ -9347,7 +9361,7 @@
       </c>
       <c r="BF75" s="11"/>
     </row>
-    <row r="76" spans="1:58">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <v>92</v>
       </c>
@@ -9413,7 +9427,7 @@
       </c>
       <c r="BF76" s="11"/>
     </row>
-    <row r="77" spans="1:58">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>58</v>
       </c>
@@ -9441,7 +9455,7 @@
       <c r="BE77" s="7"/>
       <c r="BF77" s="11"/>
     </row>
-    <row r="78" spans="1:58">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" s="11">
         <v>44</v>
       </c>
@@ -9546,7 +9560,7 @@
       </c>
       <c r="BF78" s="11"/>
     </row>
-    <row r="79" spans="1:58">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <v>55</v>
       </c>
@@ -9574,7 +9588,7 @@
       <c r="BE79" s="7"/>
       <c r="BF79" s="11"/>
     </row>
-    <row r="80" spans="1:58">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <v>43</v>
       </c>
@@ -9602,7 +9616,7 @@
       <c r="BE80" s="7"/>
       <c r="BF80" s="11"/>
     </row>
-    <row r="81" spans="1:58">
+    <row r="81" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <v>40</v>
       </c>
@@ -9707,7 +9721,7 @@
       </c>
       <c r="BF81" s="11"/>
     </row>
-    <row r="82" spans="1:58">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <v>81</v>
       </c>
@@ -9762,7 +9776,7 @@
       <c r="BE82" s="7"/>
       <c r="BF82" s="11"/>
     </row>
-    <row r="83" spans="1:58">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>81</v>
       </c>
@@ -9808,7 +9822,7 @@
       <c r="BE83" s="7"/>
       <c r="BF83" s="7"/>
     </row>
-    <row r="84" spans="1:58">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <v>59</v>
       </c>
@@ -9880,7 +9894,7 @@
       </c>
       <c r="BF84" s="11"/>
     </row>
-    <row r="85" spans="1:58">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>108</v>
       </c>
@@ -9934,7 +9948,7 @@
       </c>
       <c r="BF85"/>
     </row>
-    <row r="86" spans="1:58">
+    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>105</v>
       </c>
@@ -9961,7 +9975,7 @@
       </c>
       <c r="BF86"/>
     </row>
-    <row r="87" spans="1:58">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>62</v>
       </c>
@@ -10030,7 +10044,7 @@
       </c>
       <c r="BF87"/>
     </row>
-    <row r="88" spans="1:58">
+    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>101</v>
       </c>
@@ -10057,7 +10071,7 @@
       </c>
       <c r="BF88"/>
     </row>
-    <row r="89" spans="1:58">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>76</v>
       </c>
@@ -10129,7 +10143,7 @@
       </c>
       <c r="BF89"/>
     </row>
-    <row r="90" spans="1:58">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>76</v>
       </c>
@@ -10195,7 +10209,7 @@
       </c>
       <c r="BF90"/>
     </row>
-    <row r="91" spans="1:58">
+    <row r="91" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>76</v>
       </c>
@@ -10261,7 +10275,7 @@
       </c>
       <c r="BF91"/>
     </row>
-    <row r="92" spans="1:58">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>76</v>
       </c>
@@ -10327,7 +10341,7 @@
       </c>
       <c r="BF92"/>
     </row>
-    <row r="93" spans="1:58">
+    <row r="93" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>76</v>
       </c>
@@ -10390,7 +10404,7 @@
       </c>
       <c r="BF93"/>
     </row>
-    <row r="94" spans="1:58">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>76</v>
       </c>
@@ -10456,7 +10470,7 @@
       </c>
       <c r="BF94"/>
     </row>
-    <row r="95" spans="1:58">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>76</v>
       </c>
@@ -10522,7 +10536,7 @@
       </c>
       <c r="BF95"/>
     </row>
-    <row r="96" spans="1:58">
+    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>42</v>
       </c>
@@ -10603,7 +10617,7 @@
       </c>
       <c r="BF96"/>
     </row>
-    <row r="97" spans="1:58">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>89</v>
       </c>
@@ -10672,7 +10686,7 @@
       </c>
       <c r="BF97"/>
     </row>
-    <row r="98" spans="1:58">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>50</v>
       </c>
@@ -10798,7 +10812,7 @@
       </c>
       <c r="BF98"/>
     </row>
-    <row r="99" spans="1:58">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>50</v>
       </c>
@@ -10914,7 +10928,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="100" spans="1:58">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>112</v>
       </c>
@@ -10971,7 +10985,7 @@
       </c>
       <c r="BF100"/>
     </row>
-    <row r="101" spans="1:58">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>112</v>
       </c>
@@ -11018,7 +11032,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="102" spans="1:58">
+    <row r="102" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>70</v>
       </c>
@@ -11084,7 +11098,7 @@
       </c>
       <c r="BF102"/>
     </row>
-    <row r="103" spans="1:58">
+    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>47</v>
       </c>
@@ -11108,7 +11122,7 @@
       </c>
       <c r="BF103"/>
     </row>
-    <row r="104" spans="1:58">
+    <row r="104" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11222,7 +11236,7 @@
       </c>
       <c r="BF104"/>
     </row>
-    <row r="105" spans="1:58">
+    <row r="105" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>97</v>
       </c>
@@ -11312,7 +11326,7 @@
       </c>
       <c r="BF105"/>
     </row>
-    <row r="106" spans="1:58">
+    <row r="106" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>65</v>
       </c>
@@ -11456,7 +11470,7 @@
       </c>
       <c r="BF106"/>
     </row>
-    <row r="107" spans="1:58">
+    <row r="107" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <v>113</v>
       </c>
@@ -11528,7 +11542,7 @@
       </c>
       <c r="BF107" s="11"/>
     </row>
-    <row r="108" spans="1:58">
+    <row r="108" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
         <v>118</v>
       </c>
@@ -11612,7 +11626,7 @@
       </c>
       <c r="BF108" s="11"/>
     </row>
-    <row r="109" spans="1:58">
+    <row r="109" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>118</v>
       </c>
@@ -11690,7 +11704,7 @@
       </c>
       <c r="BF109" s="7"/>
     </row>
-    <row r="110" spans="1:58">
+    <row r="110" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>121</v>
       </c>
@@ -11762,7 +11776,7 @@
       </c>
       <c r="BF110" s="11"/>
     </row>
-    <row r="111" spans="1:58">
+    <row r="111" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <v>115</v>
       </c>
@@ -11834,7 +11848,7 @@
       </c>
       <c r="BF111" s="11"/>
     </row>
-    <row r="112" spans="1:58">
+    <row r="112" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
         <v>117</v>
       </c>
@@ -11933,7 +11947,7 @@
       </c>
       <c r="BF112" s="11"/>
     </row>
-    <row r="113" spans="1:58">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
         <v>116</v>
       </c>
@@ -12041,7 +12055,7 @@
       </c>
       <c r="BF113" s="11"/>
     </row>
-    <row r="114" spans="1:58">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A114" s="11">
         <v>123</v>
       </c>
@@ -12122,7 +12136,7 @@
       </c>
       <c r="BF114" s="11"/>
     </row>
-    <row r="115" spans="1:58">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <v>119</v>
       </c>
@@ -12203,7 +12217,7 @@
       </c>
       <c r="BF115" s="11"/>
     </row>
-    <row r="116" spans="1:58">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="11">
         <v>114</v>
       </c>
@@ -12285,7 +12299,7 @@
       </c>
       <c r="BF116" s="11"/>
     </row>
-    <row r="117" spans="1:58">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <v>114</v>
       </c>
@@ -12358,7 +12372,7 @@
       </c>
       <c r="BF117" s="11"/>
     </row>
-    <row r="118" spans="1:58">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="11">
         <v>114</v>
       </c>
@@ -12431,7 +12445,7 @@
       </c>
       <c r="BF118" s="11"/>
     </row>
-    <row r="119" spans="1:58">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>114</v>
       </c>
@@ -12504,7 +12518,7 @@
       </c>
       <c r="BF119" s="7"/>
     </row>
-    <row r="120" spans="1:58">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="11">
         <v>122</v>
       </c>
@@ -12576,7 +12590,7 @@
       </c>
       <c r="BF120" s="11"/>
     </row>
-    <row r="121" spans="1:58">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A121" s="11">
         <v>120</v>
       </c>
@@ -12622,7 +12636,7 @@
       <c r="BE121" s="7"/>
       <c r="BF121" s="11"/>
     </row>
-    <row r="122" spans="1:58">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>129</v>
       </c>
@@ -12709,7 +12723,7 @@
       </c>
       <c r="BF122"/>
     </row>
-    <row r="123" spans="1:58">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>126</v>
       </c>
@@ -12814,7 +12828,7 @@
       </c>
       <c r="BF123"/>
     </row>
-    <row r="124" spans="1:58">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>124</v>
       </c>
@@ -12895,7 +12909,7 @@
       </c>
       <c r="BF124"/>
     </row>
-    <row r="125" spans="1:58">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>131</v>
       </c>
@@ -12967,7 +12981,7 @@
       </c>
       <c r="BF125"/>
     </row>
-    <row r="126" spans="1:58">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -13057,7 +13071,7 @@
       </c>
       <c r="BF126"/>
     </row>
-    <row r="127" spans="1:58">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>127</v>
       </c>
@@ -13144,7 +13158,7 @@
       </c>
       <c r="BF127"/>
     </row>
-    <row r="128" spans="1:58">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>129</v>
       </c>
@@ -13194,9 +13208,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1042</v>
       </c>
@@ -13221,7 +13235,7 @@
       <c r="AJ1" s="9"/>
       <c r="AO1" s="4"/>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1">
+    <row r="2" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>414</v>
       </c>
@@ -13243,7 +13257,7 @@
       <c r="AJ2" s="9"/>
       <c r="AS2" s="4"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -13252,7 +13266,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -13261,7 +13275,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -13270,7 +13284,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -13279,7 +13293,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>430</v>
       </c>
@@ -13290,7 +13304,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -13301,7 +13315,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1124</v>
       </c>
@@ -13312,7 +13326,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -13323,7 +13337,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1052</v>
       </c>
@@ -13334,7 +13348,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -13345,7 +13359,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -13356,7 +13370,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -13367,7 +13381,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>494</v>
       </c>
@@ -13378,7 +13392,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>410</v>
       </c>
@@ -13389,7 +13403,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>402</v>
       </c>
@@ -13400,7 +13414,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>401</v>
       </c>
@@ -13411,7 +13425,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -13422,7 +13436,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -13433,7 +13447,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -13442,7 +13456,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -13451,7 +13465,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
@@ -13462,7 +13476,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>1072</v>
       </c>
@@ -13473,7 +13487,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>1076</v>
       </c>
@@ -13484,7 +13498,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
@@ -13495,7 +13509,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>1073</v>
       </c>
@@ -13506,7 +13520,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>1077</v>
       </c>
@@ -13517,7 +13531,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
@@ -13528,7 +13542,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1074</v>
       </c>
@@ -13539,7 +13553,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>1078</v>
       </c>
@@ -13550,7 +13564,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>17</v>
       </c>
@@ -13561,7 +13575,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
@@ -13570,7 +13584,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
@@ -13579,7 +13593,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>392</v>
       </c>
@@ -13587,7 +13601,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>393</v>
       </c>
@@ -13596,7 +13610,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>394</v>
       </c>
@@ -13605,7 +13619,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>98</v>
       </c>
@@ -13616,7 +13630,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>1093</v>
       </c>
@@ -13627,7 +13641,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1075</v>
       </c>
@@ -13636,7 +13650,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -13647,7 +13661,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>400</v>
       </c>
@@ -13658,7 +13672,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -13669,7 +13683,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>702</v>
       </c>
@@ -13680,7 +13694,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>709</v>
       </c>
@@ -13691,7 +13705,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>710</v>
       </c>
@@ -13700,7 +13714,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>706</v>
       </c>
@@ -13711,7 +13725,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>707</v>
       </c>
@@ -13720,7 +13734,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>712</v>
       </c>
@@ -13729,7 +13743,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>713</v>
       </c>
@@ -13738,7 +13752,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>714</v>
       </c>
@@ -13747,7 +13761,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>715</v>
       </c>
@@ -13756,7 +13770,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>1115</v>
       </c>
@@ -13767,7 +13781,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>1116</v>
       </c>
@@ -13778,7 +13792,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>1117</v>
       </c>
@@ -13789,7 +13803,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>1118</v>
       </c>
@@ -13800,7 +13814,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>1119</v>
       </c>
@@ -13811,7 +13825,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>1120</v>
       </c>
@@ -13835,9 +13849,9 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>909</v>
       </c>
@@ -13872,7 +13886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>910</v>
       </c>
@@ -13901,7 +13915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>911</v>
       </c>
@@ -13927,7 +13941,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>912</v>
       </c>
@@ -13957,7 +13971,7 @@
         <v>0.27927927927927926</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>913</v>
       </c>
@@ -13990,7 +14004,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>914</v>
       </c>
@@ -14019,7 +14033,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>915</v>
       </c>
@@ -14049,7 +14063,7 @@
         <v>0.17391304347826086</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>916</v>
       </c>
@@ -14081,7 +14095,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>917</v>
       </c>
@@ -14110,7 +14124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>918</v>
       </c>
@@ -14139,7 +14153,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>919</v>
       </c>
@@ -14169,7 +14183,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>920</v>
       </c>
@@ -14198,7 +14212,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>929</v>
       </c>
@@ -14227,7 +14241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>921</v>
       </c>
@@ -14256,7 +14270,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>922</v>
       </c>
@@ -14285,7 +14299,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>923</v>
       </c>
@@ -14314,7 +14328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>924</v>
       </c>
@@ -14344,7 +14358,7 @@
         <v>3.3557046979865772E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1153</v>
       </c>
@@ -14374,7 +14388,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>925</v>
       </c>
@@ -14404,7 +14418,7 @@
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>926</v>
       </c>
@@ -14434,7 +14448,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>927</v>
       </c>
@@ -14464,7 +14478,7 @@
         <v>0.11594202898550725</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>928</v>
       </c>
@@ -14493,7 +14507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>1147</v>
       </c>
@@ -14522,7 +14536,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>989</v>
       </c>
@@ -14551,7 +14565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1180</v>
       </c>
@@ -14581,7 +14595,7 @@
         <v>6.9767441860465115E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>46</v>
       </c>
@@ -14611,7 +14625,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1194</v>
       </c>
@@ -14644,7 +14658,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1187</v>
       </c>
@@ -14676,7 +14690,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>1187</v>
       </c>
@@ -14705,7 +14719,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>1187</v>
       </c>
@@ -14749,9 +14763,9 @@
       <selection activeCell="B11" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1121</v>
       </c>
@@ -14759,12 +14773,12 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -14772,7 +14786,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>942</v>
       </c>
@@ -14780,7 +14794,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -14788,7 +14802,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1124</v>
       </c>
@@ -14796,7 +14810,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -14804,7 +14818,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -14812,7 +14826,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>932</v>
       </c>
@@ -14820,7 +14834,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>931</v>
       </c>
@@ -14828,7 +14842,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -14849,18 +14863,18 @@
       <selection activeCell="B2" sqref="B2:B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="66.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="66.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>381</v>
       </c>
@@ -14888,7 +14902,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>100</v>
       </c>
@@ -14920,7 +14934,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>49</v>
       </c>
@@ -14952,7 +14966,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>60</v>
       </c>
@@ -14984,7 +14998,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>77</v>
       </c>
@@ -15014,7 +15028,7 @@
         <v>3539</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>69</v>
       </c>
@@ -15046,7 +15060,7 @@
         <v>4234</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>109</v>
       </c>
@@ -15078,7 +15092,7 @@
         <v>5638</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>46</v>
       </c>
@@ -15110,7 +15124,7 @@
         <v>6122</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>84</v>
       </c>
@@ -15142,7 +15156,7 @@
         <v>9224</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>63</v>
       </c>
@@ -15174,7 +15188,7 @@
         <v>10433</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>74</v>
       </c>
@@ -15206,7 +15220,7 @@
         <v>11099</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>107</v>
       </c>
@@ -15238,7 +15252,7 @@
         <v>12231</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>71</v>
       </c>
@@ -15270,7 +15284,7 @@
         <v>12551</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>113</v>
       </c>
@@ -15302,7 +15316,7 @@
         <v>12642</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>66</v>
       </c>
@@ -15334,7 +15348,7 @@
         <v>13436</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>53</v>
       </c>
@@ -15366,7 +15380,7 @@
         <v>13645</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>75</v>
       </c>
@@ -15398,7 +15412,7 @@
         <v>20018</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>54</v>
       </c>
@@ -15430,7 +15444,7 @@
         <v>20324</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="2" customFormat="1">
+    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>102</v>
       </c>
@@ -15458,7 +15472,7 @@
         <v>25297</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>90</v>
       </c>
@@ -15490,7 +15504,7 @@
         <v>26913</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1">
+    <row r="21" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>61</v>
       </c>
@@ -15518,7 +15532,7 @@
         <v>28649</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="2" customFormat="1">
+    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>86</v>
       </c>
@@ -15550,7 +15564,7 @@
         <v>29155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="2" customFormat="1">
+    <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>57</v>
       </c>
@@ -15580,7 +15594,7 @@
         <v>32758</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1">
+    <row r="24" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>78</v>
       </c>
@@ -15612,7 +15626,7 @@
         <v>32791</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="2" customFormat="1">
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>64</v>
       </c>
@@ -15644,7 +15658,7 @@
         <v>32959</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="2" customFormat="1">
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>68</v>
       </c>
@@ -15676,7 +15690,7 @@
         <v>34746</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="2" customFormat="1">
+    <row r="27" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>93</v>
       </c>
@@ -15708,7 +15722,7 @@
         <v>37672</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1">
+    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>48</v>
       </c>
@@ -15740,7 +15754,7 @@
         <v>38933</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="2" customFormat="1">
+    <row r="29" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>88</v>
       </c>
@@ -15772,7 +15786,7 @@
         <v>39237</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="2" customFormat="1">
+    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>111</v>
       </c>
@@ -15804,7 +15818,7 @@
         <v>39944</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="2" customFormat="1">
+    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>56</v>
       </c>
@@ -15836,7 +15850,7 @@
         <v>41100</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="2" customFormat="1">
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>82</v>
       </c>
@@ -15868,7 +15882,7 @@
         <v>41932</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="2" customFormat="1">
+    <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>104</v>
       </c>
@@ -15900,7 +15914,7 @@
         <v>46216</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="2" customFormat="1">
+    <row r="34" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>87</v>
       </c>
@@ -15930,7 +15944,7 @@
         <v>46967</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="2" customFormat="1">
+    <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>45</v>
       </c>
@@ -15962,7 +15976,7 @@
         <v>47378</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="2" customFormat="1">
+    <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>67</v>
       </c>
@@ -15994,7 +16008,7 @@
         <v>48354</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="2" customFormat="1">
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>96</v>
       </c>
@@ -16026,7 +16040,7 @@
         <v>49003</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1">
+    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>98</v>
       </c>
@@ -16058,7 +16072,7 @@
         <v>50537</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1">
+    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>79</v>
       </c>
@@ -16090,7 +16104,7 @@
         <v>50542</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="2" customFormat="1">
+    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>41</v>
       </c>
@@ -16122,7 +16136,7 @@
         <v>50721</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="2" customFormat="1">
+    <row r="41" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>106</v>
       </c>
@@ -16154,7 +16168,7 @@
         <v>51750</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="2" customFormat="1">
+    <row r="42" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>99</v>
       </c>
@@ -16186,7 +16200,7 @@
         <v>52971</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="2" customFormat="1">
+    <row r="43" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>94</v>
       </c>
@@ -16218,7 +16232,7 @@
         <v>54361</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="2" customFormat="1">
+    <row r="44" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>51</v>
       </c>
@@ -16250,7 +16264,7 @@
         <v>54775</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="2" customFormat="1">
+    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>95</v>
       </c>
@@ -16282,7 +16296,7 @@
         <v>54968</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="2" customFormat="1">
+    <row r="46" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>85</v>
       </c>
@@ -16314,7 +16328,7 @@
         <v>55220</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="2" customFormat="1">
+    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>110</v>
       </c>
@@ -16346,7 +16360,7 @@
         <v>56086</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="2" customFormat="1">
+    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>73</v>
       </c>
@@ -16378,7 +16392,7 @@
         <v>56525</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="2" customFormat="1">
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>80</v>
       </c>
@@ -16410,7 +16424,7 @@
         <v>57840</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="2" customFormat="1">
+    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>52</v>
       </c>
@@ -16442,7 +16456,7 @@
         <v>58896</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>83</v>
       </c>
@@ -16474,7 +16488,7 @@
         <v>59284</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>91</v>
       </c>
@@ -16506,7 +16520,7 @@
         <v>59320</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>72</v>
       </c>
@@ -16538,7 +16552,7 @@
         <v>60703</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>92</v>
       </c>
@@ -16570,7 +16584,7 @@
         <v>66679</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>58</v>
       </c>
@@ -16600,7 +16614,7 @@
         <v>67037</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>44</v>
       </c>
@@ -16632,7 +16646,7 @@
         <v>73767</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -16664,7 +16678,7 @@
         <v>73924</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>43</v>
       </c>
@@ -16696,7 +16710,7 @@
         <v>74887</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>40</v>
       </c>
@@ -16726,7 +16740,7 @@
         <v>75330</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>81</v>
       </c>
@@ -16756,7 +16770,7 @@
         <v>76460</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -16788,7 +16802,7 @@
         <v>78680</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>108</v>
       </c>
@@ -16820,7 +16834,7 @@
         <v>80275</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>105</v>
       </c>
@@ -16852,7 +16866,7 @@
         <v>81054</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -16884,7 +16898,7 @@
         <v>81684</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>101</v>
       </c>
@@ -16916,7 +16930,7 @@
         <v>82696</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>76</v>
       </c>
@@ -16944,7 +16958,7 @@
         <v>83890</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>42</v>
       </c>
@@ -16976,7 +16990,7 @@
         <v>84689</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>89</v>
       </c>
@@ -17008,7 +17022,7 @@
         <v>88432</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>50</v>
       </c>
@@ -17040,7 +17054,7 @@
         <v>89054</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>112</v>
       </c>
@@ -17072,7 +17086,7 @@
         <v>90316</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>70</v>
       </c>
@@ -17104,7 +17118,7 @@
         <v>92735</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>47</v>
       </c>
@@ -17136,7 +17150,7 @@
         <v>93418</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>103</v>
       </c>
@@ -17166,7 +17180,7 @@
         <v>94860</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>97</v>
       </c>
@@ -17198,7 +17212,7 @@
         <v>95244</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>65</v>
       </c>
@@ -17247,9 +17261,9 @@
       <selection activeCell="B12" activeCellId="1" sqref="B15:B21 B2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>381</v>
       </c>
@@ -17269,7 +17283,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>113</v>
       </c>
@@ -17289,7 +17303,7 @@
         <v>2.0152920465801638E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>118</v>
       </c>
@@ -17309,7 +17323,7 @@
         <v>4.674181240213704E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>121</v>
       </c>
@@ -17329,7 +17343,7 @@
         <v>0.13282679210562631</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>115</v>
       </c>
@@ -17349,7 +17363,7 @@
         <v>0.14772978119295221</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>117</v>
       </c>
@@ -17369,7 +17383,7 @@
         <v>0.19497116776968848</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>116</v>
       </c>
@@ -17389,7 +17403,7 @@
         <v>0.3082658551556392</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>123</v>
       </c>
@@ -17409,7 +17423,7 @@
         <v>0.35522680376280447</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>119</v>
       </c>
@@ -17429,7 +17443,7 @@
         <v>0.51238651611118913</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>114</v>
       </c>
@@ -17449,7 +17463,7 @@
         <v>0.79962543936843022</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>122</v>
       </c>
@@ -17469,7 +17483,7 @@
         <v>0.82351857412982277</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>120</v>
       </c>
@@ -17489,7 +17503,7 @@
         <v>0.91283573016383235</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>984</v>
       </c>
@@ -17497,7 +17511,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>130</v>
       </c>
@@ -17511,7 +17525,7 @@
         <v>4.5647988135790185E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>126</v>
       </c>
@@ -17525,7 +17539,7 @@
         <v>0.19975369256546105</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>124</v>
       </c>
@@ -17539,7 +17553,7 @@
         <v>0.38904191938792043</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>131</v>
       </c>
@@ -17553,7 +17567,7 @@
         <v>0.46913668197324998</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>125</v>
       </c>
@@ -17567,7 +17581,7 @@
         <v>0.47343686143616748</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>127</v>
       </c>
@@ -17581,7 +17595,7 @@
         <v>0.66023299344219599</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>129</v>
       </c>
@@ -17612,9 +17626,9 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>909</v>
       </c>
@@ -17625,7 +17639,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>910</v>
       </c>
@@ -17636,7 +17650,7 @@
         <v>0.11780915591189201</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>911</v>
       </c>
@@ -17647,7 +17661,7 @@
         <v>0.14190518438276789</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>912</v>
       </c>
@@ -17658,7 +17672,7 @@
         <v>0.15248178171981241</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>913</v>
       </c>
@@ -17669,7 +17683,7 @@
         <v>0.32424885057540331</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>914</v>
       </c>
@@ -17680,7 +17694,7 @@
         <v>0.36008942414901568</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>915</v>
       </c>
@@ -17691,7 +17705,7 @@
         <v>0.36473888979125946</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>916</v>
       </c>
@@ -17702,7 +17716,7 @@
         <v>0.37305006993859302</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>917</v>
       </c>
@@ -17713,7 +17727,7 @@
         <v>0.40549141682361001</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>918</v>
       </c>
@@ -17724,7 +17738,7 @@
         <v>0.49010771135660791</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>919</v>
       </c>
@@ -17735,7 +17749,7 @@
         <v>0.49766661039234461</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>920</v>
       </c>
@@ -17746,7 +17760,7 @@
         <v>0.53613889700361461</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>929</v>
       </c>
@@ -17757,7 +17771,7 @@
         <v>0.55372046150480514</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>921</v>
       </c>
@@ -17768,7 +17782,7 @@
         <v>0.56166742077086174</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>922</v>
       </c>
@@ -17779,7 +17793,7 @@
         <v>0.69538024858540026</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>923</v>
       </c>
@@ -17790,7 +17804,7 @@
         <v>0.72399036878219081</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>924</v>
       </c>
@@ -17801,7 +17815,7 @@
         <v>0.75372671693079174</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>925</v>
       </c>
@@ -17812,7 +17826,7 @@
         <v>0.90783927973393885</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>926</v>
       </c>
@@ -17823,7 +17837,7 @@
         <v>0.92374386939225039</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>927</v>
       </c>
@@ -17834,7 +17848,7 @@
         <v>0.979161553110653</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>928</v>
       </c>
@@ -17862,12 +17876,12 @@
       <selection activeCell="B1" sqref="B1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.20703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1205</v>
       </c>
@@ -17881,7 +17895,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>42989</v>
       </c>
@@ -17895,7 +17909,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>42989</v>
       </c>
@@ -17909,7 +17923,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>42989</v>
       </c>
@@ -17921,7 +17935,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>42989</v>
       </c>
@@ -17935,16 +17949,16 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
     </row>
   </sheetData>

</xml_diff>